<commit_message>
reads movies and chapters succesfully :D
</commit_message>
<xml_diff>
--- a/2do_Semestre/POO/Proyecto/videos.xlsx
+++ b/2do_Semestre/POO/Proyecto/videos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\ITC\2do_Semestre\POO\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Documents\Ubuntu\ITC\2do_Semestre\POO\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75E88C9-BF28-45E8-A819-2813DCBCDBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F79F0E-1412-4774-8FA3-C2398B0B5768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="1440" windowWidth="21600" windowHeight="11205" activeTab="1" xr2:uid="{5F935300-337B-4BAA-8EDE-4532256B092F}"/>
+    <workbookView xWindow="1898" yWindow="8438" windowWidth="16874" windowHeight="10522" activeTab="1" xr2:uid="{5F935300-337B-4BAA-8EDE-4532256B092F}"/>
   </bookViews>
   <sheets>
     <sheet name="Peliculas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="451">
   <si>
     <t>tipo</t>
   </si>
@@ -1392,7 +1392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1439,6 +1439,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1460,7 +1468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1468,6 +1476,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1784,23 +1793,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513787DD-73ED-4C36-84FD-9D2D6E4DDA2E}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="112" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="B1" zoomScale="112" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="5" width="11.5546875" style="3"/>
-    <col min="6" max="6" width="35.44140625" style="3" customWidth="1"/>
+    <col min="1" max="5" width="11.53125" style="3"/>
+    <col min="6" max="6" width="35.46484375" style="3" customWidth="1"/>
     <col min="7" max="7" width="13" style="3" customWidth="1"/>
-    <col min="8" max="9" width="11.5546875" style="3"/>
-    <col min="10" max="10" width="13.5546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" style="3"/>
+    <col min="8" max="9" width="11.53125" style="3"/>
+    <col min="10" max="10" width="13.53125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.46484375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.46484375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.53125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1882,7 +1891,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1923,7 +1932,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -2046,7 +2055,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2087,7 +2096,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -2169,7 +2178,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2210,7 +2219,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -2292,7 +2301,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -2333,7 +2342,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -2374,7 +2383,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -2415,7 +2424,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -2453,7 +2462,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -2494,7 +2503,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -2535,7 +2544,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -2576,7 +2585,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -2617,7 +2626,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -2658,7 +2667,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -2699,7 +2708,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
@@ -2740,7 +2749,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
@@ -2781,7 +2790,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
@@ -2863,7 +2872,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>18</v>
       </c>
@@ -2904,7 +2913,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
@@ -2945,7 +2954,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
@@ -2986,7 +2995,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -3027,7 +3036,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -3065,7 +3074,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -3106,7 +3115,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -3147,7 +3156,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -3188,7 +3197,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -3229,7 +3238,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -3270,7 +3279,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
@@ -3311,7 +3320,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
@@ -3349,7 +3358,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>18</v>
       </c>
@@ -3390,7 +3399,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
@@ -3513,7 +3522,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>18</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>18</v>
       </c>
@@ -3595,7 +3604,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
@@ -3636,7 +3645,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>18</v>
       </c>
@@ -3677,7 +3686,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>18</v>
       </c>
@@ -3718,7 +3727,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>18</v>
       </c>
@@ -3759,7 +3768,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>18</v>
       </c>
@@ -3800,7 +3809,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
@@ -3841,7 +3850,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>18</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>18</v>
       </c>
@@ -3923,7 +3932,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>18</v>
       </c>
@@ -3964,7 +3973,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>18</v>
       </c>
@@ -4005,7 +4014,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>18</v>
       </c>
@@ -4046,7 +4055,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>18</v>
       </c>
@@ -4087,7 +4096,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>18</v>
       </c>
@@ -4125,7 +4134,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>18</v>
       </c>
@@ -4166,7 +4175,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>18</v>
       </c>
@@ -4207,7 +4216,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>18</v>
       </c>
@@ -4248,7 +4257,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>18</v>
       </c>
@@ -4297,15 +4306,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2C3532-2D31-4090-9AAC-74914A5DF25C}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4313,40 +4322,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>286</v>
       </c>
@@ -4354,41 +4366,44 @@
         <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="6">
+        <v>83</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="6">
         <v>58</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>9.5</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="J2" s="6">
-        <v>1</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>286</v>
       </c>
@@ -4396,41 +4411,44 @@
         <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="6">
+        <v>83</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="6">
         <v>65</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>9.6999999999999993</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>1</v>
       </c>
-      <c r="K3" s="6">
+      <c r="L3" s="6">
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>286</v>
       </c>
@@ -4438,41 +4456,44 @@
         <v>63</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="6">
+        <v>83</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="6">
         <v>65</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>9.6</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>1</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <v>3</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>286</v>
       </c>
@@ -4480,41 +4501,44 @@
         <v>64</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="6">
+        <v>83</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="6">
         <v>67</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>9.5</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <v>4</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>286</v>
       </c>
@@ -4522,41 +4546,44 @@
         <v>65</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="6">
+        <v>83</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="6">
         <v>72</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>9.9</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>1</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <v>5</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>286</v>
       </c>
@@ -4564,40 +4591,43 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>287</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>290</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>87</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>282</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
         <v>289</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>286</v>
       </c>
@@ -4605,40 +4635,43 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>291</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>290</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>87</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>282</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>292</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>286</v>
       </c>
@@ -4646,40 +4679,43 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>296</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>290</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>87</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>8.4</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>282</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>3</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>295</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>286</v>
       </c>
@@ -4687,40 +4723,43 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>297</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>290</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>87</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>8.6</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>282</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>4</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>298</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>286</v>
       </c>
@@ -4728,40 +4767,43 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11">
         <v>45</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>300</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>290</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>87</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>282</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>5</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>301</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>286</v>
       </c>
@@ -4769,40 +4811,43 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12">
         <v>45</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>303</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>290</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>87</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>8.6</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>282</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>6</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>304</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>286</v>
       </c>
@@ -4810,40 +4855,43 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13">
         <v>45</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>306</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>290</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>87</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>282</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>7</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>308</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>286</v>
       </c>
@@ -4851,40 +4899,43 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14">
         <v>45</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>309</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>290</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>87</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>8.4</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>282</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>8</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>310</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>286</v>
       </c>
@@ -4892,40 +4943,43 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15">
         <v>43</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>312</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>290</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>87</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>8.5</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>282</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>9</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>313</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>286</v>
       </c>
@@ -4933,40 +4987,43 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16">
         <v>43</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>315</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>290</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>87</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>282</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>10</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>316</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>286</v>
       </c>
@@ -4974,40 +5031,43 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>318</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>290</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>87</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>9</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>282</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>1</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>11</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>324</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>286</v>
       </c>
@@ -5015,40 +5075,43 @@
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18">
         <v>45</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>320</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>290</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>87</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>8.9</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>282</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>1</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>12</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>325</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>286</v>
       </c>
@@ -5056,40 +5119,43 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19">
         <v>44</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>322</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>290</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>87</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>9.1</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>282</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>1</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>13</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>326</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>286</v>
       </c>
@@ -5097,40 +5163,43 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20">
         <v>45</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>328</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>290</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>87</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>8.9</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>282</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>1</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>14</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>327</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>286</v>
       </c>
@@ -5138,40 +5207,43 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21">
         <v>44</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>330</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>290</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>87</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>282</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>1</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>15</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>331</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>286</v>
       </c>
@@ -5179,40 +5251,43 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22">
         <v>44</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>333</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>290</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>87</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>282</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>1</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>16</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>334</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>286</v>
       </c>
@@ -5220,40 +5295,43 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23">
+        <v>83</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23">
         <v>44</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>336</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>290</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>87</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>9</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>282</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>1</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>17</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>334</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>286</v>
       </c>
@@ -5261,40 +5339,43 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24">
         <v>44</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>338</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>290</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>87</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>282</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>18</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>334</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>286</v>
       </c>
@@ -5302,40 +5383,43 @@
         <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25">
         <v>44</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>287</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>357</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>112</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>284</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
         <v>358</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>286</v>
       </c>
@@ -5343,40 +5427,43 @@
         <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26">
         <v>45</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>360</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>357</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>112</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>8.1</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>284</v>
       </c>
-      <c r="J26" s="6">
+      <c r="K26" s="6">
         <v>1</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>2</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>361</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>286</v>
       </c>
@@ -5384,40 +5471,43 @@
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27">
         <v>45</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>363</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>357</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>112</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>7.8</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>284</v>
       </c>
-      <c r="J27" s="6">
+      <c r="K27" s="6">
         <v>1</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>3</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>364</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>286</v>
       </c>
@@ -5425,40 +5515,43 @@
         <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28">
         <v>46</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>366</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>357</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>112</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>7.8</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>284</v>
       </c>
-      <c r="J28" s="6">
+      <c r="K28" s="6">
         <v>1</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>4</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>367</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>286</v>
       </c>
@@ -5466,40 +5559,43 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29">
         <v>47</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>369</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>357</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>112</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>7.8</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>284</v>
       </c>
-      <c r="J29" s="6">
+      <c r="K29" s="6">
         <v>1</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>5</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>370</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>286</v>
       </c>
@@ -5507,40 +5603,43 @@
         <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30">
         <v>43</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>372</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>357</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>112</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>8.4</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>284</v>
       </c>
-      <c r="J30" s="6">
+      <c r="K30" s="6">
         <v>1</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>6</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>374</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>286</v>
       </c>
@@ -5548,40 +5647,43 @@
         <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31">
         <v>42</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>375</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>357</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>112</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>8</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>284</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>1</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>7</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>376</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>286</v>
       </c>
@@ -5589,40 +5691,43 @@
         <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32">
+        <v>83</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32">
         <v>43</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>378</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>357</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>112</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>8</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>284</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>1</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>8</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>379</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>286</v>
       </c>
@@ -5630,40 +5735,43 @@
         <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33">
         <v>44</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>382</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>357</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>112</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>8.5</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>284</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>1</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>9</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>383</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>286</v>
       </c>
@@ -5671,40 +5779,43 @@
         <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34">
         <v>43</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>384</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>357</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>112</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>8</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>284</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>1</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>10</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>385</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5712,40 +5823,43 @@
         <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35">
         <v>43</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>387</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>357</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>112</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>8.6</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>284</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>1</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>11</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>388</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>286</v>
       </c>
@@ -5753,40 +5867,43 @@
         <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36">
         <v>41</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>390</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>357</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>112</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>8.6</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>284</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>1</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>12</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>391</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>286</v>
       </c>
@@ -5794,40 +5911,43 @@
         <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37">
         <v>43</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>393</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>357</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>112</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>6.2</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>284</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>1</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>13</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>394</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>286</v>
       </c>
@@ -5835,40 +5955,43 @@
         <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38">
+        <v>83</v>
+      </c>
+      <c r="D38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38">
         <v>41</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>396</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>357</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>112</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>7.7</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>284</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>1</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>14</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>397</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>286</v>
       </c>
@@ -5876,40 +5999,43 @@
         <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39">
         <v>42</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>399</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>357</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>112</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>7.8</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>284</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>1</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>15</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>400</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>286</v>
       </c>
@@ -5917,40 +6043,43 @@
         <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40">
+        <v>83</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40">
         <v>43</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>402</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>357</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>112</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>284</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>1</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>16</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>403</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>286</v>
       </c>
@@ -5958,40 +6087,43 @@
         <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41">
         <v>43</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>405</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>357</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>112</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>8.4</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>284</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>1</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>17</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>406</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>286</v>
       </c>
@@ -5999,40 +6131,43 @@
         <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42">
+        <v>83</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42">
         <v>40</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>408</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>357</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>112</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>284</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>1</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>18</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>409</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>286</v>
       </c>
@@ -6040,40 +6175,43 @@
         <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43">
         <v>44</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>411</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>357</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>112</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>284</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>1</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>19</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>412</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>286</v>
       </c>
@@ -6081,40 +6219,43 @@
         <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44">
         <v>44</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>414</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>357</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>112</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>284</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>1</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>20</v>
       </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
         <v>415</v>
       </c>
-      <c r="M44" t="s">
+      <c r="N44" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>286</v>
       </c>
@@ -6122,40 +6263,43 @@
         <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45">
+        <v>83</v>
+      </c>
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45">
         <v>41</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>417</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>357</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>112</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>8.6</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>284</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>1</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>21</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>418</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>286</v>
       </c>
@@ -6163,40 +6307,43 @@
         <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46">
+        <v>83</v>
+      </c>
+      <c r="D46" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46">
         <v>42</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>420</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>357</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>112</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>284</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>1</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>22</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>421</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>286</v>
       </c>
@@ -6204,40 +6351,43 @@
         <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47">
         <v>21</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>425</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>426</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>177</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>8</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>427</v>
-      </c>
-      <c r="J47">
-        <v>1</v>
       </c>
       <c r="K47">
         <v>1</v>
       </c>
-      <c r="L47" t="s">
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47" t="s">
         <v>429</v>
       </c>
-      <c r="M47" t="s">
+      <c r="N47" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>286</v>
       </c>
@@ -6245,40 +6395,43 @@
         <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48">
+        <v>101</v>
+      </c>
+      <c r="D48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48">
         <v>19</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>439</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>426</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>177</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>7.9</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>427</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>1</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>2</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>430</v>
       </c>
-      <c r="M48" t="s">
+      <c r="N48" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>286</v>
       </c>
@@ -6286,40 +6439,43 @@
         <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49">
+        <v>101</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49">
         <v>25</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>438</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>426</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>177</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>427</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>1</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>3</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
         <v>431</v>
       </c>
-      <c r="M49" t="s">
+      <c r="N49" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>286</v>
       </c>
@@ -6327,40 +6483,43 @@
         <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50">
+        <v>101</v>
+      </c>
+      <c r="D50" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50">
         <v>26</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>441</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>426</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>177</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>8.4</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>427</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>1</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>4</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>432</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>286</v>
       </c>
@@ -6368,40 +6527,43 @@
         <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51">
+        <v>101</v>
+      </c>
+      <c r="D51" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51">
         <v>24</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>443</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>426</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>177</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>427</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>1</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>5</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M51" t="s">
         <v>433</v>
       </c>
-      <c r="M51" t="s">
+      <c r="N51" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>286</v>
       </c>
@@ -6409,40 +6571,43 @@
         <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52">
+        <v>101</v>
+      </c>
+      <c r="D52" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52">
         <v>26</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>445</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>426</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>177</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>427</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>1</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>6</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>434</v>
       </c>
-      <c r="M52" t="s">
+      <c r="N52" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>286</v>
       </c>
@@ -6450,40 +6615,43 @@
         <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53">
+        <v>101</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53">
         <v>24</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>447</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>426</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>177</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>8.6</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>427</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>1</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>7</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>435</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N53" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>286</v>
       </c>
@@ -6491,38 +6659,44 @@
         <v>113</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54">
+        <v>101</v>
+      </c>
+      <c r="D54" t="s">
+        <v>68</v>
+      </c>
+      <c r="E54">
         <v>36</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>449</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>426</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>177</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>427</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>1</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>8</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>436</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N54" t="s">
         <v>450</v>
       </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E58" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -6535,13 +6709,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD42B611-CF2F-4938-8577-71DED8776207}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6561,7 +6735,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -6581,7 +6755,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -6601,7 +6775,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>279</v>
       </c>
@@ -6621,7 +6795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>279</v>
       </c>

</xml_diff>